<commit_message>
[#25] Setup for NEMSIS v3.5.0 integration, State/Agency/Facility models for Transport options, test setup
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LGI\FirstNet\Products and Services Team\CodeX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisli/Projects/natriage/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33CE5DB1-5945-44DF-9460-1604EA0DF673}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21007D3-4714-AB43-A31C-1A9E013ED796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36980" yWindow="3280" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>Age</t>
   </si>
@@ -211,6 +211,54 @@
   </si>
   <si>
     <t>PSCR Tech ToProtect Challenge</t>
+  </si>
+  <si>
+    <t> 37.767087</t>
+  </si>
+  <si>
+    <t> 37.767122</t>
+  </si>
+  <si>
+    <t> 37.767076</t>
+  </si>
+  <si>
+    <t> 37.756364</t>
+  </si>
+  <si>
+    <t> -122.406417</t>
+  </si>
+  <si>
+    <t> -122.419977</t>
+  </si>
+  <si>
+    <t> -122.419791</t>
+  </si>
+  <si>
+    <t> -122.419918</t>
+  </si>
+  <si>
+    <t> -122.421321</t>
+  </si>
+  <si>
+    <t>observations/portrait/man1.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/man2.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/woman1.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/man3.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/man4.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/woman2.jpg</t>
+  </si>
+  <si>
+    <t>observations/portrait/woman3.jpg</t>
   </si>
 </sst>
 </file>
@@ -218,9 +266,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +306,13 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -362,9 +417,10 @@
     <xf numFmtId="18" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,40 +701,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
-    <col min="10" max="10" width="8.90625" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" customWidth="1"/>
-    <col min="12" max="12" width="8.90625" customWidth="1"/>
-    <col min="13" max="13" width="21.6328125" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" customWidth="1"/>
-    <col min="17" max="17" width="9.90625" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" customWidth="1"/>
+    <col min="20" max="20" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" ht="24" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -737,7 +798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="100" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -795,8 +856,17 @@
       <c r="S4" s="13">
         <v>0.34722222222222227</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="T4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4">
+        <v>37.785834000000001</v>
+      </c>
+      <c r="V4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="98" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -844,8 +914,17 @@
       <c r="S5" s="13">
         <v>0.34236111111111112</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="137.5" x14ac:dyDescent="0.35">
+      <c r="T5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="154" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -895,8 +974,17 @@
       <c r="S6" s="13">
         <v>0.34166666666666662</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="T6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="70" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -936,8 +1024,17 @@
       <c r="S7" s="13">
         <v>0.36805555555555558</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="137.5" x14ac:dyDescent="0.35">
+      <c r="T7" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="154" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -987,8 +1084,17 @@
       <c r="S8" s="13">
         <v>0.34791666666666665</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="T8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="U8" t="s">
+        <v>65</v>
+      </c>
+      <c r="V8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="84" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -1046,8 +1152,17 @@
       <c r="S9" s="13">
         <v>0.34861111111111115</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="137.5" x14ac:dyDescent="0.35">
+      <c r="T9" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="U9">
+        <v>37.785252</v>
+      </c>
+      <c r="V9">
+        <v>-122.403587</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="154" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -1097,8 +1212,17 @@
       <c r="S10" s="13">
         <v>0.34861111111111115</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T10" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="U10">
+        <v>37.785800000000002</v>
+      </c>
+      <c r="V10">
+        <v>-122.404113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1116,7 +1240,7 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1134,7 +1258,7 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1152,7 +1276,7 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1170,7 +1294,7 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>

</xml_diff>

<commit_message>
[#45] Add Scene model and lifecycle APIs, refactor data model
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisli/Projects/natriage/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisli/Projects/peakresponse/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21007D3-4714-AB43-A31C-1A9E013ED796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49F49E0-598E-C049-AAB0-EBFB08AA07C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36980" yWindow="3280" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,25 +240,25 @@
     <t> -122.421321</t>
   </si>
   <si>
-    <t>observations/portrait/man1.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/man2.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/woman1.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/man3.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/man4.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/woman2.jpg</t>
-  </si>
-  <si>
-    <t>observations/portrait/woman3.jpg</t>
+    <t>patient-observations/portrait/man1.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/man2.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/woman1.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/man3.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/man4.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/woman2.jpg</t>
+  </si>
+  <si>
+    <t>patient-observations/portrait/woman3.jpg</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
[peakresponse/peak-ios#59] Updated Patient input form design
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisli/Projects/peakresponse/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49F49E0-598E-C049-AAB0-EBFB08AA07C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03567378-75A4-1042-88FA-31CBE99F2094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Age</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>patient-observations/portrait/woman3.jpg</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -701,13 +707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -729,17 +735,17 @@
     <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -798,7 +804,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="112" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -865,8 +871,11 @@
       <c r="V4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="98" x14ac:dyDescent="0.2">
+      <c r="W4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="98" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -923,8 +932,11 @@
       <c r="V5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="154" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="154" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -983,8 +995,11 @@
       <c r="V6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="70" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="70" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -1033,8 +1048,11 @@
       <c r="V7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="154" x14ac:dyDescent="0.2">
+      <c r="W7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="154" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -1093,8 +1111,11 @@
       <c r="V8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="84" x14ac:dyDescent="0.2">
+      <c r="W8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="84" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -1161,8 +1182,11 @@
       <c r="V9">
         <v>-122.403587</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="154" x14ac:dyDescent="0.2">
+      <c r="W9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="154" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -1221,8 +1245,11 @@
       <c r="V10">
         <v>-122.404113</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1240,7 +1267,7 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1258,7 +1285,7 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1276,7 +1303,7 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1294,7 +1321,7 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>

</xml_diff>